<commit_message>
updated the sort by difficulty
</commit_message>
<xml_diff>
--- a/website/DB.xlsx
+++ b/website/DB.xlsx
@@ -14,6 +14,9 @@
     <sheet name="6" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="Fav" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="7" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="10" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="9" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="8" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -838,19 +841,19 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
+          <t>Intermediate</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>30 Mins</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>Western</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Intermediate</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>30 Mins</t>
-        </is>
-      </c>
       <c r="F8" t="inlineStr">
         <is>
           <t>Cook the chicken breast until fully cooked, you can grill or pan-cook it with your preferred seasonings. Cook the bacon until it's crispy, then, crumble or chop it into smaller pieces. Slice the lettuce, cube the tomato, slice the onion, and slice the avocado. Warm the tortilla in a pan or microwave for a few seconds to make it pliable. Add the cooked chicken, bacon, sliced lettuce, tomato cubes, onion slices, sliced avocado, and shredded cheese to the tortilla. Drizzle ranch dressing over the ingredients. Add hot sauce according to your spice preference. Fold the sides of the tortilla towards the center and then roll it up tightly from the bottom to create a wrap.</t>
@@ -863,7 +866,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Bacon --&gt; Ham, Ranch Dressing  --&gt; Mayonnaise</t>
+          <t>Bacon --&gt; Ham, Ranch Dressing --&gt; Mayonnaise</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -888,19 +891,19 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
+          <t>Hard</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>1.5 Hours</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
           <t>Thai</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Hard</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>1.5 Hours</t>
-        </is>
-      </c>
       <c r="F9" t="inlineStr">
         <is>
           <t>In a pot, bring the chicken stock to a simmer over medium heat. Add the halved lemongrass, sliced galangal, Tom Yum chili paste, kaffir lime leaf, and halved Thai chili pepper to the simmering stock. Let it simmer for about 5-10 minutes to infuse the flavors. Add the sliced oyster mushrooms to the pot. Add the large shrimp to the pot and cook until they turn pink and opaque. Add sugar to balance the flavors. Stir in lime juice for acidity. Adjust the taste by adding more sugar, lime juice, or Tom Yum chili paste if needed. Remove the lemongrass, galangal slices, kaffir lime leaf, and Thai chili pepper halves before serving.</t>
@@ -908,7 +911,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>240 ml Chicken Stock, 0.5 Stalk Lemongrass (Halved), 0.75 Galangal (Sliced), 10 g Tom Yum Chilli Paste, 0.5 Kaffir Lime Leaf, 3 Oyster Mushrooms, 0.25 Thai Chilli Pepper (Halved), 2 Large Shrimp, 3 g Sugar, 4 ml Lime Juice, 10 g Fresh Cilantro Leaves</t>
+          <t>['240 ml Chicken Stock', '0.5 Stalk Lemongrass (Halved)', '0.75 Galangal (Sliced)', '10 g Tom Yum Chilli Paste', '0.5 Kaffir Lime Leaf', '3 Oyster Mushrooms', '0.25 Thai Chilli Pepper (Halved)', '2 Large Shrimp', '3 g Sugar', '4 ml Lime Juice', '10 g Fresh Cilantro Leaves']</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -938,17 +941,17 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
+          <t>Intermediate</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>45 Mins</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
           <t>Korean</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Intermediate</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>45 Mins</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -980,6 +983,393 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="6" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="B1" s="6" t="inlineStr">
+        <is>
+          <t>Measurement</t>
+        </is>
+      </c>
+      <c r="C1" s="6" t="inlineStr">
+        <is>
+          <t>Ingredient</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>240</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ml</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Chicken Stock'</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Stalk Lemongrass</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Galangal</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>10</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Tom Yum Chilli Paste'</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Kaffir Lime Leaf'</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Oyster Mushrooms'</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Thai Chilli Pepper</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>2</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Large Shrimp'</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>3</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Sugar'</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>4</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ml</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Lime Juice'</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Fresh Cilantro Leaves']</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="6" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="B1" s="6" t="inlineStr">
+        <is>
+          <t>Measurement</t>
+        </is>
+      </c>
+      <c r="C1" s="6" t="inlineStr">
+        <is>
+          <t>Ingredient</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Tortilla</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>20</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Chicken Breast</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>30</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Lettuce</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Slices of Bacon</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Tomato</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Onion</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Avocado</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Tablespoon Shredded Cheese</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>30</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Ranch Dressing</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Teaspoon Hot Sauce</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -2178,4 +2568,145 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="6" t="inlineStr">
+        <is>
+          <t>Quantity</t>
+        </is>
+      </c>
+      <c r="B1" s="6" t="inlineStr">
+        <is>
+          <t>Measurement</t>
+        </is>
+      </c>
+      <c r="C1" s="6" t="inlineStr">
+        <is>
+          <t>Ingredient</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Large Eggs</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>240</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ml</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Chicken Broth</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Tablespoon Light Soy Sauce</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Teaspoon Sesame Oil</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Teaspoon Salt</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>10</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Green Onions</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Teaspoon White Pepper</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>